<commit_message>
direct db upload and truncate
</commit_message>
<xml_diff>
--- a/static/Data 30.xlsx
+++ b/static/Data 30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDANT PCE\SLR FRONTEND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C2883-2ED4-4272-88CF-B412687D0BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66349EE-51F2-4710-8A54-C5DC2A21A012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30210" yWindow="1395" windowWidth="17250" windowHeight="13455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="95">
   <si>
     <t>Title</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>PCE ID</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Publication Year</t>
@@ -419,7 +416,567 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="83">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11808,20 +12365,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11832,7 +12390,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -11841,838 +12399,743 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C2" s="3">
         <v>527</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C3" s="3">
         <v>509</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C4" s="3">
         <v>489</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C5" s="3">
         <v>444</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="3">
         <v>419</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>394</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="4" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C8" s="3">
         <v>546</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C9" s="3">
         <v>545</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="4" t="b">
-        <v>1</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C10" s="3">
         <v>544</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="4" t="b">
-        <v>1</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C11" s="3">
         <v>543</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="C12" s="3">
         <v>541</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="C13" s="3">
         <v>540</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="C14" s="3">
         <v>539</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C15" s="3">
         <v>538</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="C16" s="3">
         <v>537</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C17" s="3">
         <v>536</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="C18" s="3">
         <v>533</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="C19" s="3">
         <v>532</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="C20" s="3">
         <v>530</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="C21" s="3">
         <v>528</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C22" s="3">
         <v>526</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="C23" s="3">
         <v>525</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="4" t="b">
-        <v>1</v>
-      </c>
       <c r="F23" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C24" s="3">
         <v>542</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="4" t="b">
-        <v>0</v>
-      </c>
       <c r="F24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="5" t="s">
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C25" s="3">
         <v>512</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="4" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="F25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C26" s="3">
         <v>543</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="5" t="str">
+        <v>6</v>
+      </c>
+      <c r="E26" s="5" t="str">
         <f>VLOOKUP(A26,'[1]Screening First pass'!$A:$F,3,FALSE)</f>
         <v>2008</v>
       </c>
+      <c r="F26" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="G26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C27" s="3">
         <v>490</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="F27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C28" s="3">
         <v>488</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="F28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="C29" s="3">
         <v>468</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="C30" s="3">
         <v>466</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="C31" s="3">
         <v>465</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="4" t="b">
-        <v>1</v>
-      </c>
       <c r="F31" s="5" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B7 E1:E29 B14:B29">
-    <cfRule type="containsText" dxfId="26" priority="34" operator="containsText" text="EXPO">
+  <conditionalFormatting sqref="B1:B7">
+    <cfRule type="containsText" dxfId="82" priority="35" operator="containsText" text="EXPO">
       <formula>NOT(ISERROR(SEARCH("EXPO",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="containsText" dxfId="25" priority="42" operator="containsText" text="EXPO">
+    <cfRule type="containsText" dxfId="81" priority="43" operator="containsText" text="EXPO">
       <formula>NOT(ISERROR(SEARCH("EXPO",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="duplicateValues" dxfId="24" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="36"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C7">
-    <cfRule type="duplicateValues" dxfId="21" priority="52"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C23">
-    <cfRule type="duplicateValues" dxfId="18" priority="72"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="73"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C25">
-    <cfRule type="duplicateValues" dxfId="15" priority="57"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="58"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C28">
-    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E31 B30:B31">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="EXPO">
-      <formula>NOT(ISERROR(SEARCH("EXPO",B30)))</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="62" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C31">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  <conditionalFormatting sqref="B14:B31">
+    <cfRule type="containsText" dxfId="56" priority="2" operator="containsText" text="EXPO">
+      <formula>NOT(ISERROR(SEARCH("EXPO",B14)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>